<commit_message>
2 commit - Dodanie wysyłki mailowej- ale wyskakuje Timeout error
</commit_message>
<xml_diff>
--- a/screen.xlsx
+++ b/screen.xlsx
@@ -604,7 +604,7 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1063,11 +1063,11 @@
         <v>1</v>
       </c>
       <c r="H10" s="6">
-        <v>612</v>
+        <v>750</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6">
-        <v>650</v>
+        <v>770</v>
       </c>
       <c r="K10" s="6">
         <v>1</v>

</xml_diff>